<commit_message>
Inlcuded function to produce statistical values, and rewrite the code
Still need to:
-produce Readme file
-store principle imports and exports
-quality check data by giving commodities boundary values
-if new codes become of customs data this to be flagged up
-review country classifications (am working on this and should not take long)
-review principle commodtiy classifications (working on but this is more complication problem can discuss further on Friday)
</commit_message>
<xml_diff>
--- a/data/open/OPN_FINAL_ASY_HSCodeClassifications_31-01-20.xlsx
+++ b/data/open/OPN_FINAL_ASY_HSCodeClassifications_31-01-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugopigott/Dropbox/2. Work/Repositories/vnso-RAP-tradeStats-materials/data/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDFF2A5-F697-F642-93CD-66EDD569B523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9E04FC-F663-7745-A79F-E3C72902AD09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="740" windowWidth="27640" windowHeight="15740" xr2:uid="{93478F95-04B0-5E40-892A-EBC542A6182D}"/>
+    <workbookView xWindow="780" yWindow="680" windowWidth="27640" windowHeight="15740" xr2:uid="{93478F95-04B0-5E40-892A-EBC542A6182D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>